<commit_message>
added sort to department, markTransport setup with config
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" refMode="R1C1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Марка ТЗ</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>БНП-30</t>
+  </si>
+  <si>
+    <t>Мурашко</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -409,9 +412,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -427,9 +427,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -447,9 +444,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -767,7 +761,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,261 +805,266 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
+      <c r="A2" s="33">
         <v>237</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="36">
+      <c r="A3" s="33">
         <v>238</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="29"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
+      <c r="A4" s="33">
         <v>239</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="30"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="A5" s="33">
         <v>240</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="30"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="36">
+      <c r="A6" s="33">
         <v>241</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="30"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
+      <c r="A7" s="33">
         <v>242</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="30"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="36">
+      <c r="A8" s="33">
         <v>351</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="10">
         <v>16319</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="30"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36">
+      <c r="A9" s="33">
         <v>446</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="10">
         <v>61876</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="31" t="s">
+      <c r="E9" s="31"/>
+      <c r="F9" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="35"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+      <c r="A10" s="33">
         <v>187</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="10">
         <v>17637</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="23" t="s">
+      <c r="G10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="36">
+      <c r="A11" s="33">
         <v>162</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="10">
         <v>15122</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13" t="s">
+      <c r="D11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="34">
         <v>2012309</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+      <c r="A12" s="33">
         <v>233</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="10">
         <v>15121</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="35">
         <v>2011200</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
+      <c r="A13" s="33">
         <v>334</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="39">
+      <c r="H13" s="36">
         <v>2012311</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>